<commit_message>
refact: soldierstattable 수정 (공격범위, 시야) 추가
</commit_message>
<xml_diff>
--- a/Document/GameTable/Character/SoldierStatTable.xlsx
+++ b/Document/GameTable/Character/SoldierStatTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJ\Documents\Unreal Projects\ProjectBS\Document\GameTable\Character\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7F529D-D65B-4E60-8D0D-F6A3A51B6F7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A55E33C-9AF9-4DAF-9872-27AEDAABE60D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{86F341D8-68CA-4ACF-86A3-A401C6774650}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +63,14 @@
   </si>
   <si>
     <t>HandCombatSoldier4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SightRange</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1018,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D29F918-A7B5-4A24-BBDB-528E52E83015}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1032,10 +1040,11 @@
     <col min="4" max="4" width="15.25" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="6" width="14.875" customWidth="1"/>
-    <col min="7" max="7" width="11.875" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1054,9 +1063,14 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1075,8 +1089,14 @@
       <c r="F2">
         <v>10</v>
       </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>500</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1095,8 +1115,14 @@
       <c r="F3" s="1">
         <v>10</v>
       </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>500</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1115,8 +1141,14 @@
       <c r="F4" s="1">
         <v>20</v>
       </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>500</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1134,6 +1166,12 @@
       </c>
       <c r="F5" s="1">
         <v>5</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>